<commit_message>
Recalculated table 2 stats for obesity outcome.
Realized while updating the obesity analysis script (and incorporating it into the repository) that the follow-up cap will impact each outcome separately. As such, the statistics for table 2 need to be calculated separately. Reproduced various output after making this correction.

This commit represents all of the status of work prior to the Tuesday, May 3 meeting.
</commit_message>
<xml_diff>
--- a/output/sTableB-oo-modelSummaryMedWt.xlsx
+++ b/output/sTableB-oo-modelSummaryMedWt.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="sTableB-oo-modelSummaryMedWt" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -70,7 +70,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -556,7 +556,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -908,7 +908,7 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">

</xml_diff>